<commit_message>
Rename "Customer-Import" column to "Sold-to-party"
</commit_message>
<xml_diff>
--- a/tpd/template_master_data_import.xlsx
+++ b/tpd/template_master_data_import.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jascha/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrycaj/Downloads/assets-main/tpd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC9C316-E3B1-0E4B-B725-2EC2582EB9E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07D5D18-7B5B-434D-BFC2-17BEA5A7D0A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20940" yWindow="4660" windowWidth="28800" windowHeight="16100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization-Import" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer-Import" sheetId="4" r:id="rId2"/>
+    <sheet name="Sold to Party-Import" sheetId="4" r:id="rId2"/>
     <sheet name="Delivery-Point-Import" sheetId="2" r:id="rId3"/>
     <sheet name="Scanning-Location-Import" sheetId="3" r:id="rId4"/>
     <sheet name="Route-Import" sheetId="5" r:id="rId5"/>
@@ -737,48 +737,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -794,7 +794,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1092,7 +1092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1208,7 +1208,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,9 +1374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDDDDA6-1A50-9C49-AAB9-22E3C8E9E71C}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Product import template (new fields)
</commit_message>
<xml_diff>
--- a/tpd/template_master_data_import.xlsx
+++ b/tpd/template_master_data_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrycaj/Downloads/assets-main/tpd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrycaj/osapiens_dev/TnT/assets/tpd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07D5D18-7B5B-434D-BFC2-17BEA5A7D0A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A2547-115A-F744-AFD0-84CC6C208DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,6 +39,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jascha Quintern</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{204FAA86-1106-F940-8FC9-87585A7CE16D}">
@@ -137,6 +138,330 @@
             <family val="2"/>
           </rPr>
           <t>Required (if "Outer GTIN" is not set)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{E8D30F33-C056-294E-858C-0E39EE84FC1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Notes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Type of tobacco product
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{6ECE9810-BEEF-9149-9C6E-1B3A6FD7589B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description of other type of to­bacco product</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{FB4EDFD6-152E-FF4F-B921-3100E6AE449D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Combined Nomenclature (CN) code</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="1" shapeId="0" xr:uid="{4DF5A70C-0D8F-0D4E-81F9-3D91D270553B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Average gross weight of unit packet, including packaging, in grams with 0,1 gram accuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{9E3B0150-FAFD-D345-8AAA-90755FA1062F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tobacco product identifier used in the EU-CEG system</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{23EF9F06-7901-E241-944B-1D286D961AEB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tobacco product number used in the EU-CEG system, format: NNNNN-NN-NNNNN</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{A3B5EB59-1B18-6144-820C-022DBF99539F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Intended country of retail sale, ISO Alpha-2 code</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{4F216DF6-BC26-714B-9225-2213191CC546}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Note
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Price of the smallest saleable unit</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{7830F1A6-91AB-0247-9CE4-40F2FDEE38D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Currency of the smallest unit price, ISO Alpha-3 Code</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{D8EDC57A-6F4A-EE4B-A242-648F497E4C98}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Label to be printer for the bundle price</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{F6A26DBB-8E63-7546-9616-4ADB8708713F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Notes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Label to be printer for the mastercase price</t>
         </r>
       </text>
     </comment>
@@ -145,7 +470,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -217,13 +542,49 @@
   </si>
   <si>
     <t>Mastercase GTIN</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Product Type Other</t>
+  </si>
+  <si>
+    <t>Combined Nomeclature</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>TP ID</t>
+  </si>
+  <si>
+    <t>TP PN</t>
+  </si>
+  <si>
+    <t>Intended Market</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Unit Price Currency</t>
+  </si>
+  <si>
+    <t>Bundle Price Label</t>
+  </si>
+  <si>
+    <t>Mastercase Price Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -382,6 +743,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -725,7 +1092,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -735,6 +1102,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1372,7 +1748,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDDDDA6-1A50-9C49-AAB9-22E3C8E9E71C}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1390,10 +1766,21 @@
     <col min="7" max="8" width="20.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="15.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="18.5" style="3" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1423,6 +1810,39 @@
       </c>
       <c r="J1" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1433,6 +1853,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F4998C67BB1DD4F9504D874A6E091B6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="624e1dde4addd1d33005272e700e0cbd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24afc823-56a0-4ca7-beb0-a997ee0e27fa" xmlns:ns3="d1469970-2593-4797-80af-60ba6d9ed68e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b54e602ccc85d0754d12699e144ade25" ns2:_="" ns3:_="">
     <xsd:import namespace="24afc823-56a0-4ca7-beb0-a997ee0e27fa"/>
@@ -1643,12 +2069,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1659,6 +2079,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAAE4FA-FA13-49ED-B6E0-B09773573466}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37645E6C-5CE3-454D-B85F-45887DD875EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1677,15 +2106,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAAE4FA-FA13-49ED-B6E0-B09773573466}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21283FCA-4061-4B25-BD6D-0B5DA067BA0E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added three more fields to Product template
</commit_message>
<xml_diff>
--- a/tpd/template_master_data_import.xlsx
+++ b/tpd/template_master_data_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrycaj/osapiens_dev/TnT/assets/tpd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A2547-115A-F744-AFD0-84CC6C208DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D46B45-9622-FE4F-B223-90C98BBFE193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,7 +343,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t>Intended country of retail sale, ISO Alpha-2 code</t>
         </r>
@@ -459,7 +459,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t>Label to be printer for the mastercase price</t>
         </r>
@@ -470,7 +470,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -575,6 +575,15 @@
   </si>
   <si>
     <t>Mastercase Price Label</t>
+  </si>
+  <si>
+    <t>Outer Serialization Config Key</t>
+  </si>
+  <si>
+    <t>Mastercase Serialization Config Key</t>
+  </si>
+  <si>
+    <t>Pallet Serialization Config Key</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1757,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDDDDA6-1A50-9C49-AAB9-22E3C8E9E71C}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1777,10 +1786,13 @@
     <col min="19" max="19" width="18.5" style="3" customWidth="1"/>
     <col min="20" max="20" width="17.83203125" style="3" customWidth="1"/>
     <col min="21" max="21" width="22.1640625" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="2"/>
+    <col min="22" max="22" width="25.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1843,6 +1855,15 @@
       </c>
       <c r="U1" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1853,9 +1874,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2070,19 +2094,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAAE4FA-FA13-49ED-B6E0-B09773573466}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21283FCA-4061-4B25-BD6D-0B5DA067BA0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2107,9 +2127,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21283FCA-4061-4B25-BD6D-0B5DA067BA0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAAE4FA-FA13-49ED-B6E0-B09773573466}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>